<commit_message>
[이용섭] Add - [버튼] Press, Release, Hover 델리게이트 기능 추가 Add - [WorldMapIcon] 버튼 기능 구현, WidgetSwitcher 추가 Add - [WidgetSwitcher] 래핑한 클래스 추가. Add - [SystemPopup] 분기점을 확인할수 있는 시스템 팝업 추가.
</commit_message>
<xml_diff>
--- a/Content/TableData/BasePath_Directory.xlsx
+++ b/Content/TableData/BasePath_Directory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee\Documents\Unreal Projects\ProjectCY\Content\TableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15292305-4776-4451-93AB-7517EFFCC816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E0156C-B420-46CB-A449-D0A3AF898B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{37E28BB5-F263-4C28-8728-B975D268D743}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{37E28BB5-F263-4C28-8728-B975D268D743}"/>
   </bookViews>
   <sheets>
     <sheet name="BasePath_Directory" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -168,6 +168,14 @@
   </si>
   <si>
     <t>NpcInteractionItemWidget</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SystemPopup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Widget/BuiltInWidget/SystemWidget</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -532,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DEC8D7-40B5-4EC8-A742-AFE3504F4A5A}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -607,33 +615,42 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>999</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>1000</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>10000</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>10001</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B20" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -641,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{741F188C-2F6E-4E9C-90FA-0D3BDE46E14C}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -748,6 +765,17 @@
       </c>
       <c r="C10" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1000</v>
+      </c>
+      <c r="B16">
+        <v>999</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[이용섭] Add - [MainHud] TopHudWidget 기능 추가.
[Scene] "PalWorld" 씬에서 "Title" 씬으로 이동할 수 있는 기능 추가

[Table] "Hud_TopExpander" 테이블 추가.
</commit_message>
<xml_diff>
--- a/Content/TableData/BasePath_Directory.xlsx
+++ b/Content/TableData/BasePath_Directory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee\Documents\Unreal Projects\ProjectCY\Content\TableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E0156C-B420-46CB-A449-D0A3AF898B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83696D11-C1AD-4B72-B56E-907C8CD33F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{37E28BB5-F263-4C28-8728-B975D268D743}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{37E28BB5-F263-4C28-8728-B975D268D743}"/>
   </bookViews>
   <sheets>
     <sheet name="BasePath_Directory" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -176,6 +176,30 @@
   </si>
   <si>
     <t>Widget/BuiltInWidget/SystemWidget</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MainHudWidget</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Widget/MainHud</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Widget/MainHud/Textures</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BlankImage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExitImage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Title</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -542,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DEC8D7-40B5-4EC8-A742-AFE3504F4A5A}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -613,6 +637,22 @@
       </c>
       <c r="B8" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>110</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>111</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -659,7 +699,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -758,12 +798,23 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
+        <v>100</v>
+      </c>
+      <c r="B10">
+        <v>110</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>301</v>
       </c>
-      <c r="B10">
+      <c r="B13">
         <v>10001</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C13" t="s">
         <v>31</v>
       </c>
     </row>
@@ -797,10 +848,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63CA0350-59A7-4C48-9A0B-4D64680BDFBA}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -842,18 +893,30 @@
         <v>13</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F66EDF-0680-471A-9264-F75B5A7652FA}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -948,6 +1011,34 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>111</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>111</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>